<commit_message>
funcional hasta que da clic en reproducir
</commit_message>
<xml_diff>
--- a/src/main/resources/data/search.xlsx
+++ b/src/main/resources/data/search.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROYECTOS\retoSpotify\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A31E4D-2329-4E06-91BE-DBE4422AB1A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F05E77-5E25-40B0-A38D-7EEB23E92771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25785" yWindow="975" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -33,22 +28,22 @@
     <t>password</t>
   </si>
   <si>
+    <t>validate1</t>
+  </si>
+  <si>
+    <t>song</t>
+  </si>
+  <si>
     <t>laucasj13</t>
   </si>
   <si>
     <t>Sali0313+</t>
   </si>
   <si>
-    <t>validate1</t>
-  </si>
-  <si>
-    <t>song</t>
-  </si>
-  <si>
     <t>Liked Songs</t>
   </si>
   <si>
-    <t>Diamons</t>
+    <t>Mazas y Catapultas</t>
   </si>
 </sst>
 </file>
@@ -58,7 +53,7 @@
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -104,7 +99,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -120,7 +115,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -132,7 +127,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -149,7 +144,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -179,12 +174,29 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -214,6 +226,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -369,10 +398,16 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -382,18 +417,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>

</xml_diff>